<commit_message>
time exceeded solution, will maybe come back to this one
</commit_message>
<xml_diff>
--- a/22. Generate Parentheses/Whiteboards/Solution.xlsx
+++ b/22. Generate Parentheses/Whiteboards/Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\22. Generate Parentheses\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E697CE9E-492C-4E39-A968-4C70A93F3832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3330DC1-5008-405F-A046-44F6B843D266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28950" yWindow="1935" windowWidth="24525" windowHeight="11385" activeTab="1" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="17">
   <si>
     <t>(</t>
   </si>
@@ -45,6 +45,48 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>(((())))</t>
+  </si>
+  <si>
+    <t>((()()))</t>
+  </si>
+  <si>
+    <t>((())())</t>
+  </si>
+  <si>
+    <t>((()))()</t>
+  </si>
+  <si>
+    <t>(()(()))</t>
+  </si>
+  <si>
+    <t>(()()())</t>
+  </si>
+  <si>
+    <t>(()())()</t>
+  </si>
+  <si>
+    <t>(())(())</t>
+  </si>
+  <si>
+    <t>(())()()</t>
+  </si>
+  <si>
+    <t>()((()))</t>
+  </si>
+  <si>
+    <t>()(()())</t>
+  </si>
+  <si>
+    <t>()(())()</t>
+  </si>
+  <si>
+    <t>()()(())</t>
+  </si>
+  <si>
+    <t>()()()()</t>
   </si>
 </sst>
 </file>
@@ -435,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="G4:AJ23"/>
+  <dimension ref="G4:AU23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD9" sqref="X9:AD9"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -446,7 +488,7 @@
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W4" s="1">
         <v>0</v>
       </c>
@@ -472,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="X5" s="1">
         <v>1</v>
       </c>
@@ -492,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="3" t="s">
         <v>0</v>
       </c>
@@ -556,8 +598,40 @@
       <c r="AJ6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL6" s="1">
+        <f>IF(W6="(",W$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AM6" s="1">
+        <f t="shared" ref="AM6:AU19" si="0">IF(X6="(",X$4,"")</f>
+        <v>1</v>
+      </c>
+      <c r="AN6" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO6" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G7" s="3" t="s">
         <v>0</v>
       </c>
@@ -621,8 +695,44 @@
       <c r="AJ7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL7" s="1">
+        <f t="shared" ref="AL7:AL19" si="1">IF(W7="(",W$4,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN7" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP7" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G8" s="3" t="s">
         <v>0</v>
       </c>
@@ -686,8 +796,48 @@
       <c r="AJ8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN8" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ8" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AR8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G9" s="3" t="s">
         <v>0</v>
       </c>
@@ -751,8 +901,48 @@
       <c r="AJ9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN9" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR9" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AS9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G10" s="3" t="s">
         <v>0</v>
       </c>
@@ -816,8 +1006,48 @@
       <c r="AJ10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AO10" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J11" s="1" t="s">
         <v>2</v>
       </c>
@@ -854,8 +1084,48 @@
       <c r="AJ11" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AO11" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ11" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AR11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W12" s="4" t="s">
         <v>0</v>
       </c>
@@ -889,8 +1159,48 @@
       <c r="AJ12" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AO12" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR12" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AS12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W13" s="4" t="s">
         <v>0</v>
       </c>
@@ -924,8 +1234,48 @@
       <c r="AJ13" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AO13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ13" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AR13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W14" s="4" t="s">
         <v>0</v>
       </c>
@@ -959,8 +1309,48 @@
       <c r="AJ14" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AN14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AO14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP14" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR14" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AS14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W15" s="4" t="s">
         <v>0</v>
       </c>
@@ -985,8 +1375,48 @@
       <c r="AD15" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="7:36" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL15" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AN15" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO15" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP15" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="7:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W16" s="4" t="s">
         <v>0</v>
       </c>
@@ -1011,8 +1441,48 @@
       <c r="AD16" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AN16" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO16" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ16" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AR16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1037,8 +1507,48 @@
       <c r="AD17" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL17" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AN17" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO17" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AP17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AQ17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR17" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AS17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W18" s="4" t="s">
         <v>0</v>
       </c>
@@ -1066,8 +1576,48 @@
       <c r="AI18" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL18" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AN18" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP18" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ18" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="AR18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AS18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W19" s="4" t="s">
         <v>0</v>
       </c>
@@ -1092,8 +1642,48 @@
       <c r="AD19" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AM19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AN19" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AO19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AP19" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="AQ19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AR19" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AS19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AT19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AU19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N21" s="4" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N22" s="4" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="14:35" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="14:47" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N23" s="4" t="s">
         <v>0</v>
       </c>
@@ -1187,12 +1777,443 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44A32BA-2E78-40A3-AD4F-C0D1A186A5C0}">
-  <dimension ref="A1"/>
+  <dimension ref="D8:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="8" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" t="str">
+        <f>VLOOKUP(E8,$F$8:$F$24,1,FALSE)</f>
+        <v>(((())))</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="str">
+        <f>VLOOKUP(K8,$L$8:$L$24,1,FALSE)</f>
+        <v>(((())))</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" ref="H9:H24" si="0">VLOOKUP(E9,$F$8:$F$24,1,FALSE)</f>
+        <v>((()()))</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" ref="N9:N24" si="1">VLOOKUP(K9,$L$8:$L$24,1,FALSE)</f>
+        <v>((()()))</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>((())())</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>((())())</v>
+      </c>
+    </row>
+    <row r="11" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>((()))()</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>((()))()</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>(()(()))</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>(()(()))</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>(()()())</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>(()()())</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>(()())()</v>
+      </c>
+      <c r="J14">
+        <v>7</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>(()())()</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>(())(())</v>
+      </c>
+      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="1"/>
+        <v>(())(())</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>(())()()</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="1"/>
+        <v>(())()()</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>()((()))</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="1"/>
+        <v>()((()))</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>()(()())</v>
+      </c>
+      <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="1"/>
+        <v>()(()())</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>()(())()</v>
+      </c>
+      <c r="J19">
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="1"/>
+        <v>()(())()</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>()()(())</v>
+      </c>
+      <c r="J20">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>()()(())</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>()()()()</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L21" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="1"/>
+        <v>()()()()</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <v>15</v>
+      </c>
+      <c r="N22" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>16</v>
+      </c>
+      <c r="N23" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="J24">
+        <v>17</v>
+      </c>
+      <c r="N24" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>